<commit_message>
Fixed & finished players logic
</commit_message>
<xml_diff>
--- a/src/data/F1 2024 Predictor.xlsx
+++ b/src/data/F1 2024 Predictor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a582e4c3d66e654a/Documents/1. Aaron Personal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jamescrawley/Desktop/f1-2024/src/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="576" documentId="8_{7CF4B238-9409-4FEA-A226-8B5B499172BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF028173-77D0-46A3-B742-470651E7CB74}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAAFB183-0FE6-444E-9206-B926B9C294B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{3F9DE8E9-65F2-47CB-BC88-20A9FB558031}"/>
+    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" activeTab="1" xr2:uid="{3F9DE8E9-65F2-47CB-BC88-20A9FB558031}"/>
   </bookViews>
   <sheets>
     <sheet name="Collated Scores" sheetId="1" r:id="rId1"/>
@@ -515,16 +515,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -534,6 +525,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -859,17 +859,17 @@
       <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="17.625" customWidth="1"/>
-    <col min="3" max="3" width="14.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="5" max="5" width="7.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="12.5" customWidth="1"/>
-    <col min="11" max="11" width="17.625" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
@@ -889,10 +889,10 @@
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B5" s="2">
         <f>Races!F125</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C5" s="2" t="str" cm="1">
         <f t="array" ref="C5:C21">TRANSPOSE(_xlfn._xlws.FILTER(Races!E2:AL2, Races!E2:AL2&lt;&gt;""))</f>
@@ -915,17 +915,17 @@
       </c>
       <c r="K5" s="2" t="str">
         <f>IFERROR(VLOOKUP(L5,$B$5:$C$98,2,FALSE),0)</f>
-        <v>Harrison Reeve</v>
+        <v>Sam Cartledge</v>
       </c>
       <c r="L5">
         <f>MAX(B5:B42)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B6" s="2">
         <f>Races!H125</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="str">
         <v>Alex Withero</v>
@@ -944,17 +944,17 @@
       </c>
       <c r="K6" s="2" t="str">
         <f>IFERROR(VLOOKUP(L6,$B$5:$C$98,2,FALSE),0)</f>
-        <v>Chloe Freer</v>
+        <v>Cam Burgess</v>
       </c>
       <c r="L6">
         <f>IF(COUNT(B5:B98)=0, 0, LARGE(B5:B98, 2))</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B7" s="2">
         <f>Races!J125</f>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="C7" s="2" t="str">
         <v>Cam Burgess</v>
@@ -977,17 +977,17 @@
       </c>
       <c r="K7" s="2" t="str">
         <f>IFERROR(VLOOKUP(L7,$B$5:$C$98,2,FALSE),0)</f>
-        <v>Chloe Freer</v>
+        <v>Cam Burgess</v>
       </c>
       <c r="L7">
         <f>IF(COUNT($B$5:$B$98)=0, 0, LARGE($B$5:$B$98, 3))</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B8" s="2">
         <f>Races!L125</f>
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="C8" s="2" t="str">
         <v>Chloe Freer</v>
@@ -998,10 +998,10 @@
       <c r="J8" s="2"/>
       <c r="K8" s="2"/>
     </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B9" s="2">
         <f>Races!N125</f>
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="C9" s="2" t="str">
         <v>Harrison Reeve</v>
@@ -1019,10 +1019,10 @@
       <c r="J9" s="2"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B10" s="2">
         <f>Races!P125</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C10" s="2" t="str">
         <v>James Robinson</v>
@@ -1033,10 +1033,10 @@
       <c r="J10" s="2"/>
       <c r="K10" s="2"/>
     </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B11" s="2">
         <f>Races!R125</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C11" s="2" t="str">
         <v>James Crawley</v>
@@ -1054,10 +1054,10 @@
       <c r="J11" s="2"/>
       <c r="K11" s="2"/>
     </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B12" s="2">
         <f>Races!T125</f>
-        <v>5</v>
+        <v>25</v>
       </c>
       <c r="C12" s="2" t="str">
         <v>El May</v>
@@ -1068,10 +1068,10 @@
       <c r="J12" s="2"/>
       <c r="K12" s="2"/>
     </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B13" s="2">
         <f>Races!V125</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C13" s="2" t="str">
         <v>Louie Cochrane</v>
@@ -1082,10 +1082,10 @@
       <c r="J13" s="2"/>
       <c r="K13" s="2"/>
     </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B14" s="2">
         <f>Races!X125</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C14" s="2" t="str">
         <v>Luke Reeves</v>
@@ -1093,10 +1093,10 @@
       <c r="J14" s="2"/>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B15" s="2">
         <f>Races!Z125</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C15" s="2" t="str">
         <v>Fin Tapp</v>
@@ -1107,10 +1107,10 @@
       <c r="J15" s="2"/>
       <c r="K15" s="2"/>
     </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:12" x14ac:dyDescent="0.15">
       <c r="B16" s="2">
         <f>Races!AB125</f>
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="C16" s="2" t="str">
         <v>Sam Cartledge</v>
@@ -1121,10 +1121,10 @@
       <c r="J16" s="2"/>
       <c r="K16" s="2"/>
     </row>
-    <row r="17" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B17" s="2">
         <f>Races!AD125</f>
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="C17" s="2" t="str">
         <v>Matt Hyett</v>
@@ -1135,10 +1135,10 @@
       <c r="J17" s="2"/>
       <c r="K17" s="2"/>
     </row>
-    <row r="18" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B18" s="2">
         <f>Races!AF125</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C18" s="2" t="str">
         <v>Scott Benninson</v>
@@ -1147,10 +1147,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B19" s="2">
         <f>Races!AH125</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="C19" s="2" t="str">
         <v>Ollie McCann</v>
@@ -1159,10 +1159,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B20" s="2">
         <f>Races!AJ125</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="C20" s="2" t="str">
         <v>Owen Millet</v>
@@ -1171,10 +1171,10 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B21" s="2">
         <f>Races!AL125</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C21" s="2" t="str">
         <v>Matt Watson</v>
@@ -1183,27 +1183,27 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
     </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
     </row>
-    <row r="25" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
     </row>
-    <row r="26" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
     </row>
-    <row r="27" spans="2:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:11" x14ac:dyDescent="0.15">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
     </row>
@@ -1225,186 +1225,186 @@
   </sheetPr>
   <dimension ref="A1:AM128"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="174" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="4" ySplit="3" topLeftCell="E4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="F1" sqref="F1"/>
       <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
-      <selection pane="bottomRight" sqref="A1:AL13"/>
+      <selection pane="bottomRight" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="4.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.83203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17" customWidth="1"/>
     <col min="5" max="5" width="10" customWidth="1"/>
-    <col min="6" max="6" width="5.625" customWidth="1"/>
+    <col min="6" max="6" width="5.6640625" customWidth="1"/>
     <col min="7" max="7" width="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" customWidth="1"/>
-    <col min="16" max="16" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="10" customWidth="1"/>
-    <col min="20" max="20" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="10" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="10" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="10" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="10" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="10" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="10" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="37" max="37" width="10" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="5.625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="6.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="A1" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="D1" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-    </row>
-    <row r="2" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="14" t="s">
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
+      <c r="AC1" s="12"/>
+      <c r="AD1" s="12"/>
+      <c r="AE1" s="12"/>
+      <c r="AF1" s="12"/>
+      <c r="AG1" s="12"/>
+      <c r="AH1" s="12"/>
+      <c r="AI1" s="12"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+    </row>
+    <row r="2" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="12"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="17"/>
+      <c r="G2" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="15"/>
-      <c r="I2" s="14" t="s">
+      <c r="H2" s="17"/>
+      <c r="I2" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="J2" s="15"/>
-      <c r="K2" s="14" t="s">
+      <c r="J2" s="17"/>
+      <c r="K2" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="14" t="s">
+      <c r="L2" s="17"/>
+      <c r="M2" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="N2" s="15"/>
-      <c r="O2" s="14" t="s">
+      <c r="N2" s="17"/>
+      <c r="O2" s="16" t="s">
         <v>52</v>
       </c>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="14" t="s">
+      <c r="P2" s="17"/>
+      <c r="Q2" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="R2" s="15"/>
-      <c r="S2" s="14" t="s">
+      <c r="R2" s="17"/>
+      <c r="S2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="14" t="s">
+      <c r="T2" s="17"/>
+      <c r="U2" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="V2" s="15"/>
-      <c r="W2" s="14" t="s">
+      <c r="V2" s="17"/>
+      <c r="W2" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="14" t="s">
+      <c r="X2" s="17"/>
+      <c r="Y2" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="14" t="s">
+      <c r="Z2" s="17"/>
+      <c r="AA2" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="14" t="s">
+      <c r="AB2" s="17"/>
+      <c r="AC2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="14" t="s">
+      <c r="AD2" s="17"/>
+      <c r="AE2" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="14" t="s">
+      <c r="AF2" s="17"/>
+      <c r="AG2" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="14" t="s">
+      <c r="AH2" s="17"/>
+      <c r="AI2" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="14" t="s">
+      <c r="AJ2" s="17"/>
+      <c r="AK2" s="16" t="s">
         <v>97</v>
       </c>
-      <c r="AL2" s="15"/>
+      <c r="AL2" s="17"/>
       <c r="AM2" s="7"/>
     </row>
-    <row r="3" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
+    <row r="3" spans="1:39" s="6" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="12"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
       <c r="E3" s="9" t="s">
         <v>9</v>
       </c>
@@ -1509,11 +1509,11 @@
       </c>
       <c r="AM3" s="7"/>
     </row>
-    <row r="4" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="13">
+    <row r="4" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="12">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>14</v>
       </c>
       <c r="C4" s="8" t="s">
@@ -1642,9 +1642,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="13"/>
-      <c r="B5" s="13"/>
+    <row r="5" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
       <c r="C5" s="8" t="s">
         <v>41</v>
       </c>
@@ -1771,9 +1771,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="13"/>
-      <c r="B6" s="13"/>
+    <row r="6" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="12"/>
+      <c r="B6" s="12"/>
       <c r="C6" s="8" t="s">
         <v>46</v>
       </c>
@@ -1900,9 +1900,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
+    <row r="7" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="12"/>
+      <c r="B7" s="12"/>
       <c r="C7" s="8" t="s">
         <v>12</v>
       </c>
@@ -2029,9 +2029,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
+    <row r="8" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="12"/>
+      <c r="B8" s="12"/>
       <c r="C8" s="8" t="s">
         <v>42</v>
       </c>
@@ -2158,25 +2158,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13">
+    <row r="9" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="12">
         <v>2</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="12" t="s">
         <v>63</v>
       </c>
       <c r="C9" s="8" t="s">
         <v>18</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F9" s="8">
         <f>IF(E9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G9" s="8" t="s">
         <v>23</v>
@@ -2190,251 +2190,251 @@
       </c>
       <c r="J9" s="8">
         <f>IF(I9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L9" s="8">
         <f>IF(K9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N9" s="8">
         <f>IF(M9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="P9" s="8">
         <f>IF(O9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="R9" s="8">
         <f>IF(Q9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="T9" s="8">
         <f>IF(S9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="V9" s="8">
         <f>IF(U9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="X9" s="8">
         <f>IF(W9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="Z9" s="8">
         <f>IF(Y9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AB9" s="8">
         <f>IF(AA9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AD9" s="8">
         <f>IF(AC9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AF9" s="8">
         <f>IF(AE9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AH9" s="8">
         <f>IF(AG9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AJ9" s="8">
         <f>IF(AI9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK9" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AL9" s="8">
         <f>IF(AK9=$D9,Data!$D$3,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
       <c r="C10" s="8" t="s">
         <v>41</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>45</v>
+        <v>19</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="F10" s="8">
         <f>IF(E10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="H10" s="8">
         <f>IF(G10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="I10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="J10" s="8">
         <f>IF(I10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="L10" s="8">
         <f>IF(K10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="M10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N10" s="8">
         <f>IF(M10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="O10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="P10" s="8">
         <f>IF(O10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Q10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="R10" s="8">
         <f>IF(Q10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="T10" s="8">
         <f>IF(S10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="U10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="V10" s="8">
         <f>IF(U10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="W10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="X10" s="8">
         <f>IF(W10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="Z10" s="8">
         <f>IF(Y10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AB10" s="8">
         <f>IF(AA10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AC10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AD10" s="8">
         <f>IF(AC10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AE10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AF10" s="8">
         <f>IF(AE10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AG10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AH10" s="8">
         <f>IF(AG10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AI10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AJ10" s="8">
         <f>IF(AI10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK10" s="8" t="s">
         <v>19</v>
       </c>
       <c r="AL10" s="8">
         <f>IF(AK10=$D10,Data!$D$4,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="12"/>
+      <c r="B11" s="12"/>
       <c r="C11" s="8" t="s">
         <v>46</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="F11" s="8">
         <f>IF(E11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="G11" s="8" t="s">
         <v>94</v>
@@ -2448,7 +2448,7 @@
       </c>
       <c r="J11" s="8">
         <f>IF(I11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>94</v>
@@ -2476,7 +2476,7 @@
       </c>
       <c r="R11" s="8">
         <f>IF(Q11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="S11" s="8" t="s">
         <v>92</v>
@@ -2497,14 +2497,14 @@
       </c>
       <c r="X11" s="8">
         <f>IF(W11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="Z11" s="8">
         <f>IF(Y11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AA11" s="8" t="s">
         <v>86</v>
@@ -2539,24 +2539,24 @@
       </c>
       <c r="AJ11" s="8">
         <f>IF(AI11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="AK11" s="8" t="s">
         <v>88</v>
       </c>
       <c r="AL11" s="8">
         <f>IF(AK11=$D11,Data!$D$5,0)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A12" s="12"/>
+      <c r="B12" s="12"/>
       <c r="C12" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>45</v>
+        <v>23</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>19</v>
@@ -2612,7 +2612,7 @@
       </c>
       <c r="T12" s="8">
         <f>IF(S12=$D12,Data!$D$6,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="U12" s="8" t="s">
         <v>26</v>
@@ -2678,14 +2678,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="13"/>
+    <row r="13" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A13" s="12"/>
+      <c r="B13" s="12"/>
       <c r="C13" s="8" t="s">
         <v>42</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>38</v>
@@ -2706,7 +2706,7 @@
       </c>
       <c r="J13" s="8">
         <f>IF(I13=$D13,Data!$D$7,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K13" s="8" t="s">
         <v>20</v>
@@ -2769,7 +2769,7 @@
       </c>
       <c r="AB13" s="8">
         <f>IF(AA13=$D13,Data!$D$7,0)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AC13" s="8" t="s">
         <v>38</v>
@@ -2807,11 +2807,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="13">
+    <row r="14" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A14" s="12">
         <v>3</v>
       </c>
-      <c r="B14" s="13" t="s">
+      <c r="B14" s="12" t="s">
         <v>64</v>
       </c>
       <c r="C14" s="8" t="s">
@@ -2906,9 +2906,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="13"/>
-      <c r="B15" s="13"/>
+    <row r="15" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A15" s="12"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="8" t="s">
         <v>41</v>
       </c>
@@ -3001,9 +3001,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="13"/>
-      <c r="B16" s="13"/>
+    <row r="16" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A16" s="12"/>
+      <c r="B16" s="12"/>
       <c r="C16" s="8" t="s">
         <v>46</v>
       </c>
@@ -3096,9 +3096,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="13"/>
-      <c r="B17" s="13"/>
+    <row r="17" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A17" s="12"/>
+      <c r="B17" s="12"/>
       <c r="C17" s="8" t="s">
         <v>12</v>
       </c>
@@ -3191,9 +3191,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="13"/>
-      <c r="B18" s="13"/>
+    <row r="18" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A18" s="12"/>
+      <c r="B18" s="12"/>
       <c r="C18" s="8" t="s">
         <v>42</v>
       </c>
@@ -3286,11 +3286,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="13">
+    <row r="19" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A19" s="12">
         <v>4</v>
       </c>
-      <c r="B19" s="13" t="s">
+      <c r="B19" s="12" t="s">
         <v>65</v>
       </c>
       <c r="C19" s="8" t="s">
@@ -3385,9 +3385,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="13"/>
-      <c r="B20" s="13"/>
+    <row r="20" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A20" s="12"/>
+      <c r="B20" s="12"/>
       <c r="C20" s="8" t="s">
         <v>41</v>
       </c>
@@ -3480,9 +3480,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13"/>
-      <c r="B21" s="13"/>
+    <row r="21" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A21" s="12"/>
+      <c r="B21" s="12"/>
       <c r="C21" s="8" t="s">
         <v>46</v>
       </c>
@@ -3575,9 +3575,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="13"/>
-      <c r="B22" s="13"/>
+    <row r="22" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A22" s="12"/>
+      <c r="B22" s="12"/>
       <c r="C22" s="8" t="s">
         <v>12</v>
       </c>
@@ -3670,9 +3670,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="13"/>
-      <c r="B23" s="13"/>
+    <row r="23" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A23" s="12"/>
+      <c r="B23" s="12"/>
       <c r="C23" s="8" t="s">
         <v>42</v>
       </c>
@@ -3765,11 +3765,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="13">
+    <row r="24" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A24" s="12">
         <v>5</v>
       </c>
-      <c r="B24" s="13" t="s">
+      <c r="B24" s="12" t="s">
         <v>66</v>
       </c>
       <c r="C24" s="8" t="s">
@@ -3864,9 +3864,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="13"/>
-      <c r="B25" s="13"/>
+    <row r="25" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A25" s="12"/>
+      <c r="B25" s="12"/>
       <c r="C25" s="8" t="s">
         <v>41</v>
       </c>
@@ -3959,9 +3959,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13"/>
-      <c r="B26" s="13"/>
+    <row r="26" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A26" s="12"/>
+      <c r="B26" s="12"/>
       <c r="C26" s="8" t="s">
         <v>46</v>
       </c>
@@ -4054,9 +4054,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="13"/>
-      <c r="B27" s="13"/>
+    <row r="27" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A27" s="12"/>
+      <c r="B27" s="12"/>
       <c r="C27" s="8" t="s">
         <v>12</v>
       </c>
@@ -4149,9 +4149,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="13"/>
-      <c r="B28" s="13"/>
+    <row r="28" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A28" s="12"/>
+      <c r="B28" s="12"/>
       <c r="C28" s="8" t="s">
         <v>42</v>
       </c>
@@ -4244,11 +4244,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="13">
+    <row r="29" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A29" s="12">
         <v>6</v>
       </c>
-      <c r="B29" s="13" t="s">
+      <c r="B29" s="12" t="s">
         <v>67</v>
       </c>
       <c r="C29" s="8" t="s">
@@ -4343,9 +4343,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13"/>
-      <c r="B30" s="13"/>
+    <row r="30" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A30" s="12"/>
+      <c r="B30" s="12"/>
       <c r="C30" s="8" t="s">
         <v>41</v>
       </c>
@@ -4438,9 +4438,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="13"/>
-      <c r="B31" s="13"/>
+    <row r="31" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A31" s="12"/>
+      <c r="B31" s="12"/>
       <c r="C31" s="8" t="s">
         <v>46</v>
       </c>
@@ -4533,9 +4533,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="13"/>
-      <c r="B32" s="13"/>
+    <row r="32" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A32" s="12"/>
+      <c r="B32" s="12"/>
       <c r="C32" s="8" t="s">
         <v>12</v>
       </c>
@@ -4628,9 +4628,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13"/>
-      <c r="B33" s="13"/>
+    <row r="33" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A33" s="12"/>
+      <c r="B33" s="12"/>
       <c r="C33" s="8" t="s">
         <v>42</v>
       </c>
@@ -4723,11 +4723,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="13">
+    <row r="34" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A34" s="12">
         <v>7</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="12" t="s">
         <v>68</v>
       </c>
       <c r="C34" s="8" t="s">
@@ -4822,9 +4822,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="35" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="13"/>
-      <c r="B35" s="13"/>
+    <row r="35" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A35" s="12"/>
+      <c r="B35" s="12"/>
       <c r="C35" s="8" t="s">
         <v>41</v>
       </c>
@@ -4917,9 +4917,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="13"/>
-      <c r="B36" s="13"/>
+    <row r="36" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A36" s="12"/>
+      <c r="B36" s="12"/>
       <c r="C36" s="8" t="s">
         <v>46</v>
       </c>
@@ -5012,9 +5012,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13"/>
-      <c r="B37" s="13"/>
+    <row r="37" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A37" s="12"/>
+      <c r="B37" s="12"/>
       <c r="C37" s="8" t="s">
         <v>12</v>
       </c>
@@ -5107,9 +5107,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="13"/>
-      <c r="B38" s="13"/>
+    <row r="38" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A38" s="12"/>
+      <c r="B38" s="12"/>
       <c r="C38" s="8" t="s">
         <v>42</v>
       </c>
@@ -5202,11 +5202,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="13">
+    <row r="39" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A39" s="12">
         <v>8</v>
       </c>
-      <c r="B39" s="13" t="s">
+      <c r="B39" s="12" t="s">
         <v>76</v>
       </c>
       <c r="C39" s="8" t="s">
@@ -5301,9 +5301,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="13"/>
-      <c r="B40" s="13"/>
+    <row r="40" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A40" s="12"/>
+      <c r="B40" s="12"/>
       <c r="C40" s="8" t="s">
         <v>41</v>
       </c>
@@ -5396,9 +5396,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="13"/>
-      <c r="B41" s="13"/>
+    <row r="41" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A41" s="12"/>
+      <c r="B41" s="12"/>
       <c r="C41" s="8" t="s">
         <v>46</v>
       </c>
@@ -5491,9 +5491,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="13"/>
-      <c r="B42" s="13"/>
+    <row r="42" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A42" s="12"/>
+      <c r="B42" s="12"/>
       <c r="C42" s="8" t="s">
         <v>12</v>
       </c>
@@ -5586,9 +5586,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="13"/>
-      <c r="B43" s="13"/>
+    <row r="43" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A43" s="12"/>
+      <c r="B43" s="12"/>
       <c r="C43" s="8" t="s">
         <v>42</v>
       </c>
@@ -5681,11 +5681,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="13">
+    <row r="44" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A44" s="12">
         <v>9</v>
       </c>
-      <c r="B44" s="13" t="s">
+      <c r="B44" s="12" t="s">
         <v>77</v>
       </c>
       <c r="C44" s="8" t="s">
@@ -5780,9 +5780,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="13"/>
-      <c r="B45" s="13"/>
+    <row r="45" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A45" s="12"/>
+      <c r="B45" s="12"/>
       <c r="C45" s="8" t="s">
         <v>41</v>
       </c>
@@ -5875,9 +5875,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="13"/>
-      <c r="B46" s="13"/>
+    <row r="46" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A46" s="12"/>
+      <c r="B46" s="12"/>
       <c r="C46" s="8" t="s">
         <v>46</v>
       </c>
@@ -5970,9 +5970,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="13"/>
-      <c r="B47" s="13"/>
+    <row r="47" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A47" s="12"/>
+      <c r="B47" s="12"/>
       <c r="C47" s="8" t="s">
         <v>12</v>
       </c>
@@ -6065,9 +6065,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="13"/>
-      <c r="B48" s="13"/>
+    <row r="48" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A48" s="12"/>
+      <c r="B48" s="12"/>
       <c r="C48" s="8" t="s">
         <v>42</v>
       </c>
@@ -6160,11 +6160,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="13">
+    <row r="49" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A49" s="12">
         <v>10</v>
       </c>
-      <c r="B49" s="13" t="s">
+      <c r="B49" s="12" t="s">
         <v>78</v>
       </c>
       <c r="C49" s="8" t="s">
@@ -6259,9 +6259,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="13"/>
-      <c r="B50" s="13"/>
+    <row r="50" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A50" s="12"/>
+      <c r="B50" s="12"/>
       <c r="C50" s="8" t="s">
         <v>41</v>
       </c>
@@ -6354,9 +6354,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="13"/>
-      <c r="B51" s="13"/>
+    <row r="51" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A51" s="12"/>
+      <c r="B51" s="12"/>
       <c r="C51" s="8" t="s">
         <v>46</v>
       </c>
@@ -6449,9 +6449,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="13"/>
-      <c r="B52" s="13"/>
+    <row r="52" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A52" s="12"/>
+      <c r="B52" s="12"/>
       <c r="C52" s="8" t="s">
         <v>12</v>
       </c>
@@ -6544,9 +6544,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="13"/>
-      <c r="B53" s="13"/>
+    <row r="53" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A53" s="12"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="8" t="s">
         <v>42</v>
       </c>
@@ -6639,11 +6639,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="13">
+    <row r="54" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A54" s="12">
         <v>11</v>
       </c>
-      <c r="B54" s="13" t="s">
+      <c r="B54" s="12" t="s">
         <v>79</v>
       </c>
       <c r="C54" s="8" t="s">
@@ -6738,9 +6738,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="13"/>
-      <c r="B55" s="13"/>
+    <row r="55" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="12"/>
+      <c r="B55" s="12"/>
       <c r="C55" s="8" t="s">
         <v>41</v>
       </c>
@@ -6833,9 +6833,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="13"/>
-      <c r="B56" s="13"/>
+    <row r="56" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="12"/>
+      <c r="B56" s="12"/>
       <c r="C56" s="8" t="s">
         <v>46</v>
       </c>
@@ -6928,9 +6928,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="57" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="13"/>
-      <c r="B57" s="13"/>
+    <row r="57" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="12"/>
+      <c r="B57" s="12"/>
       <c r="C57" s="8" t="s">
         <v>12</v>
       </c>
@@ -7023,9 +7023,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="13"/>
-      <c r="B58" s="13"/>
+    <row r="58" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="12"/>
+      <c r="B58" s="12"/>
       <c r="C58" s="8" t="s">
         <v>42</v>
       </c>
@@ -7118,11 +7118,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="59" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="13">
+    <row r="59" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="12">
         <v>12</v>
       </c>
-      <c r="B59" s="13" t="s">
+      <c r="B59" s="12" t="s">
         <v>80</v>
       </c>
       <c r="C59" s="8" t="s">
@@ -7217,9 +7217,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="13"/>
-      <c r="B60" s="13"/>
+    <row r="60" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="12"/>
+      <c r="B60" s="12"/>
       <c r="C60" s="8" t="s">
         <v>41</v>
       </c>
@@ -7312,9 +7312,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="13"/>
-      <c r="B61" s="13"/>
+    <row r="61" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A61" s="12"/>
+      <c r="B61" s="12"/>
       <c r="C61" s="8" t="s">
         <v>46</v>
       </c>
@@ -7407,9 +7407,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="13"/>
-      <c r="B62" s="13"/>
+    <row r="62" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A62" s="12"/>
+      <c r="B62" s="12"/>
       <c r="C62" s="8" t="s">
         <v>12</v>
       </c>
@@ -7502,9 +7502,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="13"/>
-      <c r="B63" s="13"/>
+    <row r="63" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A63" s="12"/>
+      <c r="B63" s="12"/>
       <c r="C63" s="8" t="s">
         <v>42</v>
       </c>
@@ -7597,11 +7597,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="13">
+    <row r="64" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A64" s="12">
         <v>13</v>
       </c>
-      <c r="B64" s="13" t="s">
+      <c r="B64" s="12" t="s">
         <v>85</v>
       </c>
       <c r="C64" s="8" t="s">
@@ -7696,9 +7696,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="13"/>
-      <c r="B65" s="13"/>
+    <row r="65" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A65" s="12"/>
+      <c r="B65" s="12"/>
       <c r="C65" s="8" t="s">
         <v>41</v>
       </c>
@@ -7791,9 +7791,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="13"/>
-      <c r="B66" s="13"/>
+    <row r="66" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A66" s="12"/>
+      <c r="B66" s="12"/>
       <c r="C66" s="8" t="s">
         <v>46</v>
       </c>
@@ -7886,9 +7886,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="13"/>
-      <c r="B67" s="13"/>
+    <row r="67" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A67" s="12"/>
+      <c r="B67" s="12"/>
       <c r="C67" s="8" t="s">
         <v>12</v>
       </c>
@@ -7981,9 +7981,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="13"/>
-      <c r="B68" s="13"/>
+    <row r="68" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A68" s="12"/>
+      <c r="B68" s="12"/>
       <c r="C68" s="8" t="s">
         <v>42</v>
       </c>
@@ -8076,11 +8076,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="13">
+    <row r="69" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A69" s="12">
         <v>14</v>
       </c>
-      <c r="B69" s="13" t="s">
+      <c r="B69" s="12" t="s">
         <v>81</v>
       </c>
       <c r="C69" s="8" t="s">
@@ -8175,9 +8175,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="13"/>
-      <c r="B70" s="13"/>
+    <row r="70" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A70" s="12"/>
+      <c r="B70" s="12"/>
       <c r="C70" s="8" t="s">
         <v>41</v>
       </c>
@@ -8270,9 +8270,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="71" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="13"/>
-      <c r="B71" s="13"/>
+    <row r="71" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A71" s="12"/>
+      <c r="B71" s="12"/>
       <c r="C71" s="8" t="s">
         <v>46</v>
       </c>
@@ -8365,9 +8365,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="13"/>
-      <c r="B72" s="13"/>
+    <row r="72" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A72" s="12"/>
+      <c r="B72" s="12"/>
       <c r="C72" s="8" t="s">
         <v>12</v>
       </c>
@@ -8460,9 +8460,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="73" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="13"/>
-      <c r="B73" s="13"/>
+    <row r="73" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A73" s="12"/>
+      <c r="B73" s="12"/>
       <c r="C73" s="8" t="s">
         <v>42</v>
       </c>
@@ -8555,11 +8555,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="74" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A74" s="13">
+    <row r="74" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A74" s="12">
         <v>15</v>
       </c>
-      <c r="B74" s="16" t="s">
+      <c r="B74" s="13" t="s">
         <v>82</v>
       </c>
       <c r="C74" s="8" t="s">
@@ -8654,9 +8654,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="75" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="13"/>
-      <c r="B75" s="17"/>
+    <row r="75" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A75" s="12"/>
+      <c r="B75" s="14"/>
       <c r="C75" s="8" t="s">
         <v>41</v>
       </c>
@@ -8749,9 +8749,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="76" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A76" s="13"/>
-      <c r="B76" s="17"/>
+    <row r="76" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A76" s="12"/>
+      <c r="B76" s="14"/>
       <c r="C76" s="8" t="s">
         <v>46</v>
       </c>
@@ -8844,9 +8844,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A77" s="13"/>
-      <c r="B77" s="17"/>
+    <row r="77" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A77" s="12"/>
+      <c r="B77" s="14"/>
       <c r="C77" s="8" t="s">
         <v>12</v>
       </c>
@@ -8939,9 +8939,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="78" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A78" s="13"/>
-      <c r="B78" s="18"/>
+    <row r="78" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A78" s="12"/>
+      <c r="B78" s="15"/>
       <c r="C78" s="8" t="s">
         <v>42</v>
       </c>
@@ -9034,11 +9034,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="79" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A79" s="13">
+    <row r="79" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A79" s="12">
         <v>16</v>
       </c>
-      <c r="B79" s="16" t="s">
+      <c r="B79" s="13" t="s">
         <v>83</v>
       </c>
       <c r="C79" s="8" t="s">
@@ -9133,9 +9133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A80" s="13"/>
-      <c r="B80" s="17"/>
+    <row r="80" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A80" s="12"/>
+      <c r="B80" s="14"/>
       <c r="C80" s="8" t="s">
         <v>41</v>
       </c>
@@ -9228,9 +9228,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="81" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A81" s="13"/>
-      <c r="B81" s="17"/>
+    <row r="81" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A81" s="12"/>
+      <c r="B81" s="14"/>
       <c r="C81" s="8" t="s">
         <v>46</v>
       </c>
@@ -9323,9 +9323,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A82" s="13"/>
-      <c r="B82" s="17"/>
+    <row r="82" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A82" s="12"/>
+      <c r="B82" s="14"/>
       <c r="C82" s="8" t="s">
         <v>12</v>
       </c>
@@ -9418,9 +9418,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A83" s="13"/>
-      <c r="B83" s="18"/>
+    <row r="83" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A83" s="12"/>
+      <c r="B83" s="15"/>
       <c r="C83" s="8" t="s">
         <v>42</v>
       </c>
@@ -9513,11 +9513,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="84" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A84" s="13">
+    <row r="84" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A84" s="12">
         <v>17</v>
       </c>
-      <c r="B84" s="16" t="s">
+      <c r="B84" s="13" t="s">
         <v>69</v>
       </c>
       <c r="C84" s="8" t="s">
@@ -9612,9 +9612,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="85" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A85" s="13"/>
-      <c r="B85" s="17"/>
+    <row r="85" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A85" s="12"/>
+      <c r="B85" s="14"/>
       <c r="C85" s="8" t="s">
         <v>41</v>
       </c>
@@ -9707,9 +9707,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A86" s="13"/>
-      <c r="B86" s="17"/>
+    <row r="86" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A86" s="12"/>
+      <c r="B86" s="14"/>
       <c r="C86" s="8" t="s">
         <v>46</v>
       </c>
@@ -9802,9 +9802,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A87" s="13"/>
-      <c r="B87" s="17"/>
+    <row r="87" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A87" s="12"/>
+      <c r="B87" s="14"/>
       <c r="C87" s="8" t="s">
         <v>12</v>
       </c>
@@ -9897,9 +9897,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A88" s="13"/>
-      <c r="B88" s="18"/>
+    <row r="88" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A88" s="12"/>
+      <c r="B88" s="15"/>
       <c r="C88" s="8" t="s">
         <v>42</v>
       </c>
@@ -9992,11 +9992,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A89" s="13">
+    <row r="89" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A89" s="12">
         <v>18</v>
       </c>
-      <c r="B89" s="16" t="s">
+      <c r="B89" s="13" t="s">
         <v>70</v>
       </c>
       <c r="C89" s="8" t="s">
@@ -10091,9 +10091,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="13"/>
-      <c r="B90" s="17"/>
+    <row r="90" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A90" s="12"/>
+      <c r="B90" s="14"/>
       <c r="C90" s="8" t="s">
         <v>41</v>
       </c>
@@ -10186,9 +10186,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A91" s="13"/>
-      <c r="B91" s="17"/>
+    <row r="91" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A91" s="12"/>
+      <c r="B91" s="14"/>
       <c r="C91" s="8" t="s">
         <v>46</v>
       </c>
@@ -10281,9 +10281,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A92" s="13"/>
-      <c r="B92" s="17"/>
+    <row r="92" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A92" s="12"/>
+      <c r="B92" s="14"/>
       <c r="C92" s="8" t="s">
         <v>12</v>
       </c>
@@ -10376,9 +10376,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A93" s="13"/>
-      <c r="B93" s="18"/>
+    <row r="93" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A93" s="12"/>
+      <c r="B93" s="15"/>
       <c r="C93" s="8" t="s">
         <v>42</v>
       </c>
@@ -10471,11 +10471,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A94" s="13">
+    <row r="94" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A94" s="12">
         <v>19</v>
       </c>
-      <c r="B94" s="16" t="s">
+      <c r="B94" s="13" t="s">
         <v>71</v>
       </c>
       <c r="C94" s="8" t="s">
@@ -10570,9 +10570,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A95" s="13"/>
-      <c r="B95" s="17"/>
+    <row r="95" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A95" s="12"/>
+      <c r="B95" s="14"/>
       <c r="C95" s="8" t="s">
         <v>41</v>
       </c>
@@ -10665,9 +10665,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A96" s="13"/>
-      <c r="B96" s="17"/>
+    <row r="96" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A96" s="12"/>
+      <c r="B96" s="14"/>
       <c r="C96" s="8" t="s">
         <v>46</v>
       </c>
@@ -10760,9 +10760,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="97" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A97" s="13"/>
-      <c r="B97" s="17"/>
+    <row r="97" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A97" s="12"/>
+      <c r="B97" s="14"/>
       <c r="C97" s="8" t="s">
         <v>12</v>
       </c>
@@ -10855,9 +10855,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="98" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A98" s="13"/>
-      <c r="B98" s="18"/>
+    <row r="98" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A98" s="12"/>
+      <c r="B98" s="15"/>
       <c r="C98" s="8" t="s">
         <v>42</v>
       </c>
@@ -10950,11 +10950,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="99" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A99" s="13">
+    <row r="99" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A99" s="12">
         <v>20</v>
       </c>
-      <c r="B99" s="16" t="s">
+      <c r="B99" s="13" t="s">
         <v>72</v>
       </c>
       <c r="C99" s="8" t="s">
@@ -11049,9 +11049,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="100" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="13"/>
-      <c r="B100" s="17"/>
+    <row r="100" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A100" s="12"/>
+      <c r="B100" s="14"/>
       <c r="C100" s="8" t="s">
         <v>41</v>
       </c>
@@ -11144,9 +11144,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="101" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A101" s="13"/>
-      <c r="B101" s="17"/>
+    <row r="101" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A101" s="12"/>
+      <c r="B101" s="14"/>
       <c r="C101" s="8" t="s">
         <v>46</v>
       </c>
@@ -11239,9 +11239,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="102" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A102" s="13"/>
-      <c r="B102" s="17"/>
+    <row r="102" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A102" s="12"/>
+      <c r="B102" s="14"/>
       <c r="C102" s="8" t="s">
         <v>12</v>
       </c>
@@ -11334,9 +11334,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="103" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A103" s="13"/>
-      <c r="B103" s="18"/>
+    <row r="103" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A103" s="12"/>
+      <c r="B103" s="15"/>
       <c r="C103" s="8" t="s">
         <v>42</v>
       </c>
@@ -11429,11 +11429,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="104" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A104" s="13">
+    <row r="104" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A104" s="12">
         <v>21</v>
       </c>
-      <c r="B104" s="16" t="s">
+      <c r="B104" s="13" t="s">
         <v>73</v>
       </c>
       <c r="C104" s="8" t="s">
@@ -11528,9 +11528,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A105" s="13"/>
-      <c r="B105" s="17"/>
+    <row r="105" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A105" s="12"/>
+      <c r="B105" s="14"/>
       <c r="C105" s="8" t="s">
         <v>41</v>
       </c>
@@ -11623,9 +11623,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A106" s="13"/>
-      <c r="B106" s="17"/>
+    <row r="106" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A106" s="12"/>
+      <c r="B106" s="14"/>
       <c r="C106" s="8" t="s">
         <v>46</v>
       </c>
@@ -11718,9 +11718,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A107" s="13"/>
-      <c r="B107" s="17"/>
+    <row r="107" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A107" s="12"/>
+      <c r="B107" s="14"/>
       <c r="C107" s="8" t="s">
         <v>12</v>
       </c>
@@ -11813,9 +11813,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A108" s="13"/>
-      <c r="B108" s="18"/>
+    <row r="108" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A108" s="12"/>
+      <c r="B108" s="15"/>
       <c r="C108" s="8" t="s">
         <v>42</v>
       </c>
@@ -11908,11 +11908,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A109" s="13">
+    <row r="109" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A109" s="12">
         <v>22</v>
       </c>
-      <c r="B109" s="16" t="s">
+      <c r="B109" s="13" t="s">
         <v>74</v>
       </c>
       <c r="C109" s="8" t="s">
@@ -12007,9 +12007,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A110" s="13"/>
-      <c r="B110" s="17"/>
+    <row r="110" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A110" s="12"/>
+      <c r="B110" s="14"/>
       <c r="C110" s="8" t="s">
         <v>41</v>
       </c>
@@ -12102,9 +12102,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A111" s="13"/>
-      <c r="B111" s="17"/>
+    <row r="111" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A111" s="12"/>
+      <c r="B111" s="14"/>
       <c r="C111" s="8" t="s">
         <v>46</v>
       </c>
@@ -12197,9 +12197,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A112" s="13"/>
-      <c r="B112" s="17"/>
+    <row r="112" spans="1:38" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A112" s="12"/>
+      <c r="B112" s="14"/>
       <c r="C112" s="8" t="s">
         <v>12</v>
       </c>
@@ -12292,9 +12292,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A113" s="13"/>
-      <c r="B113" s="18"/>
+    <row r="113" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A113" s="12"/>
+      <c r="B113" s="15"/>
       <c r="C113" s="8" t="s">
         <v>42</v>
       </c>
@@ -12387,11 +12387,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A114" s="13">
+    <row r="114" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A114" s="12">
         <v>23</v>
       </c>
-      <c r="B114" s="16" t="s">
+      <c r="B114" s="13" t="s">
         <v>75</v>
       </c>
       <c r="C114" s="8" t="s">
@@ -12486,9 +12486,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A115" s="13"/>
-      <c r="B115" s="17"/>
+    <row r="115" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A115" s="12"/>
+      <c r="B115" s="14"/>
       <c r="C115" s="8" t="s">
         <v>41</v>
       </c>
@@ -12581,9 +12581,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="116" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A116" s="13"/>
-      <c r="B116" s="17"/>
+    <row r="116" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A116" s="12"/>
+      <c r="B116" s="14"/>
       <c r="C116" s="8" t="s">
         <v>46</v>
       </c>
@@ -12676,9 +12676,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="117" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A117" s="13"/>
-      <c r="B117" s="17"/>
+    <row r="117" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A117" s="12"/>
+      <c r="B117" s="14"/>
       <c r="C117" s="8" t="s">
         <v>12</v>
       </c>
@@ -12771,9 +12771,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A118" s="13"/>
-      <c r="B118" s="18"/>
+    <row r="118" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A118" s="12"/>
+      <c r="B118" s="15"/>
       <c r="C118" s="8" t="s">
         <v>42</v>
       </c>
@@ -12866,11 +12866,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="119" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A119" s="13">
+    <row r="119" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A119" s="12">
         <v>24</v>
       </c>
-      <c r="B119" s="16" t="s">
+      <c r="B119" s="13" t="s">
         <v>84</v>
       </c>
       <c r="C119" s="8" t="s">
@@ -12965,9 +12965,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="120" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A120" s="13"/>
-      <c r="B120" s="17"/>
+    <row r="120" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A120" s="12"/>
+      <c r="B120" s="14"/>
       <c r="C120" s="8" t="s">
         <v>41</v>
       </c>
@@ -13060,9 +13060,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A121" s="13"/>
-      <c r="B121" s="17"/>
+    <row r="121" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A121" s="12"/>
+      <c r="B121" s="14"/>
       <c r="C121" s="8" t="s">
         <v>46</v>
       </c>
@@ -13155,9 +13155,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A122" s="13"/>
-      <c r="B122" s="17"/>
+    <row r="122" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A122" s="12"/>
+      <c r="B122" s="14"/>
       <c r="C122" s="8" t="s">
         <v>12</v>
       </c>
@@ -13250,9 +13250,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A123" s="13"/>
-      <c r="B123" s="18"/>
+    <row r="123" spans="1:39" s="10" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="A123" s="12"/>
+      <c r="B123" s="15"/>
       <c r="C123" s="8" t="s">
         <v>42</v>
       </c>
@@ -13345,176 +13345,176 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B125" s="12" t="s">
+    <row r="125" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="B125" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="C125" s="12"/>
-      <c r="F125" s="12">
+      <c r="C125" s="18"/>
+      <c r="F125" s="18">
         <f>SUM(F4:F123)</f>
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="G125" s="6"/>
-      <c r="H125" s="12">
+      <c r="H125" s="18">
         <f>SUM(H4:H123)</f>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="I125" s="6"/>
-      <c r="J125" s="12">
+      <c r="J125" s="18">
         <f>SUM(J4:J123)</f>
-        <v>10</v>
+        <v>35</v>
       </c>
       <c r="K125" s="6"/>
-      <c r="L125" s="12">
+      <c r="L125" s="18">
         <f>SUM(L4:L123)</f>
+        <v>30</v>
+      </c>
+      <c r="M125" s="6"/>
+      <c r="N125" s="18">
+        <f>SUM(N4:N123)</f>
+        <v>35</v>
+      </c>
+      <c r="O125" s="6"/>
+      <c r="P125" s="18">
+        <f>SUM(P4:P123)</f>
         <v>20</v>
       </c>
-      <c r="M125" s="6"/>
-      <c r="N125" s="12">
-        <f>SUM(N4:N123)</f>
+      <c r="Q125" s="6"/>
+      <c r="R125" s="18">
+        <f>SUM(R4:R123)</f>
+        <v>35</v>
+      </c>
+      <c r="S125" s="6"/>
+      <c r="T125" s="18">
+        <f>SUM(T4:T123)</f>
         <v>25</v>
       </c>
-      <c r="O125" s="6"/>
-      <c r="P125" s="12">
-        <f>SUM(P4:P123)</f>
-        <v>10</v>
-      </c>
-      <c r="Q125" s="6"/>
-      <c r="R125" s="12">
-        <f>SUM(R4:R123)</f>
+      <c r="U125" s="6"/>
+      <c r="V125" s="18">
+        <f>SUM(V4:V123)</f>
         <v>20</v>
       </c>
-      <c r="S125" s="6"/>
-      <c r="T125" s="12">
-        <f>SUM(T4:T123)</f>
-        <v>5</v>
-      </c>
-      <c r="U125" s="6"/>
-      <c r="V125" s="12">
-        <f>SUM(V4:V123)</f>
-        <v>10</v>
-      </c>
       <c r="W125" s="6"/>
-      <c r="X125" s="12">
+      <c r="X125" s="18">
         <f>SUM(X4:X123)</f>
+        <v>35</v>
+      </c>
+      <c r="Y125" s="6"/>
+      <c r="Z125" s="18">
+        <f>SUM(Z4:Z123)</f>
+        <v>35</v>
+      </c>
+      <c r="AA125" s="6"/>
+      <c r="AB125" s="18">
+        <f>SUM(AB4:AB123)</f>
+        <v>40</v>
+      </c>
+      <c r="AC125" s="6"/>
+      <c r="AD125" s="18">
+        <f>SUM(AD4:AD123)</f>
         <v>20</v>
       </c>
-      <c r="Y125" s="6"/>
-      <c r="Z125" s="12">
-        <f>SUM(Z4:Z123)</f>
-        <v>20</v>
-      </c>
-      <c r="AA125" s="6"/>
-      <c r="AB125" s="12">
-        <f>SUM(AB4:AB123)</f>
-        <v>20</v>
-      </c>
-      <c r="AC125" s="6"/>
-      <c r="AD125" s="12">
-        <f>SUM(AD4:AD123)</f>
-        <v>10</v>
-      </c>
       <c r="AE125" s="6"/>
-      <c r="AF125" s="12">
+      <c r="AF125" s="18">
         <f>SUM(AF4:AF123)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AG125" s="6"/>
-      <c r="AH125" s="12">
+      <c r="AH125" s="18">
         <f>SUM(AH4:AH123)</f>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="AI125" s="6"/>
-      <c r="AJ125" s="12">
+      <c r="AJ125" s="18">
         <f>SUM(AJ4:AJ123)</f>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="AK125" s="6"/>
-      <c r="AL125" s="12">
+      <c r="AL125" s="18">
         <f>SUM(AL4:AL123)</f>
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="AM125" s="7"/>
     </row>
-    <row r="126" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B126" s="12"/>
-      <c r="C126" s="12"/>
-      <c r="F126" s="12"/>
+    <row r="126" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="B126" s="18"/>
+      <c r="C126" s="18"/>
+      <c r="F126" s="18"/>
       <c r="G126" s="6"/>
-      <c r="H126" s="12"/>
+      <c r="H126" s="18"/>
       <c r="I126" s="6"/>
-      <c r="J126" s="12"/>
+      <c r="J126" s="18"/>
       <c r="K126" s="6"/>
-      <c r="L126" s="12"/>
+      <c r="L126" s="18"/>
       <c r="M126" s="6"/>
-      <c r="N126" s="12"/>
+      <c r="N126" s="18"/>
       <c r="O126" s="6"/>
-      <c r="P126" s="12"/>
+      <c r="P126" s="18"/>
       <c r="Q126" s="6"/>
-      <c r="R126" s="12"/>
+      <c r="R126" s="18"/>
       <c r="S126" s="6"/>
-      <c r="T126" s="12"/>
+      <c r="T126" s="18"/>
       <c r="U126" s="6"/>
-      <c r="V126" s="12"/>
+      <c r="V126" s="18"/>
       <c r="W126" s="6"/>
-      <c r="X126" s="12"/>
+      <c r="X126" s="18"/>
       <c r="Y126" s="6"/>
-      <c r="Z126" s="12"/>
+      <c r="Z126" s="18"/>
       <c r="AA126" s="6"/>
-      <c r="AB126" s="12"/>
+      <c r="AB126" s="18"/>
       <c r="AC126" s="6"/>
-      <c r="AD126" s="12"/>
+      <c r="AD126" s="18"/>
       <c r="AE126" s="6"/>
-      <c r="AF126" s="12"/>
+      <c r="AF126" s="18"/>
       <c r="AG126" s="6"/>
-      <c r="AH126" s="12"/>
+      <c r="AH126" s="18"/>
       <c r="AI126" s="6"/>
-      <c r="AJ126" s="12"/>
+      <c r="AJ126" s="18"/>
       <c r="AK126" s="6"/>
-      <c r="AL126" s="12"/>
+      <c r="AL126" s="18"/>
       <c r="AM126" s="7"/>
     </row>
-    <row r="127" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B127" s="12"/>
-      <c r="C127" s="12"/>
-      <c r="F127" s="12"/>
+    <row r="127" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="B127" s="18"/>
+      <c r="C127" s="18"/>
+      <c r="F127" s="18"/>
       <c r="G127" s="6"/>
-      <c r="H127" s="12"/>
+      <c r="H127" s="18"/>
       <c r="I127" s="6"/>
-      <c r="J127" s="12"/>
+      <c r="J127" s="18"/>
       <c r="K127" s="6"/>
-      <c r="L127" s="12"/>
+      <c r="L127" s="18"/>
       <c r="M127" s="6"/>
-      <c r="N127" s="12"/>
+      <c r="N127" s="18"/>
       <c r="O127" s="6"/>
-      <c r="P127" s="12"/>
+      <c r="P127" s="18"/>
       <c r="Q127" s="6"/>
-      <c r="R127" s="12"/>
+      <c r="R127" s="18"/>
       <c r="S127" s="6"/>
-      <c r="T127" s="12"/>
+      <c r="T127" s="18"/>
       <c r="U127" s="6"/>
-      <c r="V127" s="12"/>
+      <c r="V127" s="18"/>
       <c r="W127" s="6"/>
-      <c r="X127" s="12"/>
+      <c r="X127" s="18"/>
       <c r="Y127" s="6"/>
-      <c r="Z127" s="12"/>
+      <c r="Z127" s="18"/>
       <c r="AA127" s="6"/>
-      <c r="AB127" s="12"/>
+      <c r="AB127" s="18"/>
       <c r="AC127" s="6"/>
-      <c r="AD127" s="12"/>
+      <c r="AD127" s="18"/>
       <c r="AE127" s="6"/>
-      <c r="AF127" s="12"/>
+      <c r="AF127" s="18"/>
       <c r="AG127" s="6"/>
-      <c r="AH127" s="12"/>
+      <c r="AH127" s="18"/>
       <c r="AI127" s="6"/>
-      <c r="AJ127" s="12"/>
+      <c r="AJ127" s="18"/>
       <c r="AK127" s="6"/>
-      <c r="AL127" s="12"/>
+      <c r="AL127" s="18"/>
       <c r="AM127" s="7"/>
     </row>
-    <row r="128" spans="1:39" x14ac:dyDescent="0.2">
-      <c r="B128" s="12"/>
-      <c r="C128" s="12"/>
+    <row r="128" spans="1:39" x14ac:dyDescent="0.15">
+      <c r="B128" s="18"/>
+      <c r="C128" s="18"/>
       <c r="Y128" s="2"/>
     </row>
   </sheetData>
@@ -13555,6 +13555,78 @@
     <filterColumn colId="37" showButton="0"/>
   </autoFilter>
   <mergeCells count="88">
+    <mergeCell ref="AF125:AF127"/>
+    <mergeCell ref="AH125:AH127"/>
+    <mergeCell ref="AJ125:AJ127"/>
+    <mergeCell ref="AL125:AL127"/>
+    <mergeCell ref="AD125:AD127"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="U2:V2"/>
+    <mergeCell ref="B125:C128"/>
+    <mergeCell ref="Z125:Z127"/>
+    <mergeCell ref="AB125:AB127"/>
+    <mergeCell ref="F125:F127"/>
+    <mergeCell ref="H125:H127"/>
+    <mergeCell ref="J125:J127"/>
+    <mergeCell ref="T125:T127"/>
+    <mergeCell ref="P125:P127"/>
+    <mergeCell ref="R125:R127"/>
+    <mergeCell ref="L125:L127"/>
+    <mergeCell ref="N125:N127"/>
+    <mergeCell ref="V125:V127"/>
+    <mergeCell ref="X125:X127"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="Y2:Z2"/>
+    <mergeCell ref="W2:X2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="AE2:AF2"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AI2:AJ2"/>
+    <mergeCell ref="D1:D3"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="E1:AL1"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="AC2:AD2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="Q2:R2"/>
+    <mergeCell ref="A34:A38"/>
+    <mergeCell ref="B34:B38"/>
+    <mergeCell ref="A39:A43"/>
+    <mergeCell ref="B39:B43"/>
+    <mergeCell ref="A9:A13"/>
+    <mergeCell ref="B9:B13"/>
+    <mergeCell ref="A14:A18"/>
+    <mergeCell ref="B14:B18"/>
+    <mergeCell ref="A24:A28"/>
+    <mergeCell ref="B24:B28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="B29:B33"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="A44:A48"/>
+    <mergeCell ref="B44:B48"/>
+    <mergeCell ref="A49:A53"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="A54:A58"/>
+    <mergeCell ref="B54:B58"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="B84:B88"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B89:B93"/>
+    <mergeCell ref="A59:A63"/>
+    <mergeCell ref="B59:B63"/>
+    <mergeCell ref="A69:A73"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="A74:A78"/>
+    <mergeCell ref="B74:B78"/>
     <mergeCell ref="A119:A123"/>
     <mergeCell ref="A64:A68"/>
     <mergeCell ref="B64:B68"/>
@@ -13571,78 +13643,6 @@
     <mergeCell ref="B104:B108"/>
     <mergeCell ref="A79:A83"/>
     <mergeCell ref="B79:B83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="B84:B88"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B89:B93"/>
-    <mergeCell ref="A59:A63"/>
-    <mergeCell ref="B59:B63"/>
-    <mergeCell ref="A69:A73"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="A74:A78"/>
-    <mergeCell ref="B74:B78"/>
-    <mergeCell ref="A44:A48"/>
-    <mergeCell ref="B44:B48"/>
-    <mergeCell ref="A49:A53"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="A54:A58"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="A34:A38"/>
-    <mergeCell ref="B34:B38"/>
-    <mergeCell ref="A39:A43"/>
-    <mergeCell ref="B39:B43"/>
-    <mergeCell ref="A9:A13"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="A14:A18"/>
-    <mergeCell ref="B14:B18"/>
-    <mergeCell ref="A24:A28"/>
-    <mergeCell ref="B24:B28"/>
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="B29:B33"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="Q2:R2"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="Y2:Z2"/>
-    <mergeCell ref="W2:X2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="AE2:AF2"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AI2:AJ2"/>
-    <mergeCell ref="D1:D3"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="S2:T2"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="E1:AL1"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="AC2:AD2"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="U2:V2"/>
-    <mergeCell ref="B125:C128"/>
-    <mergeCell ref="Z125:Z127"/>
-    <mergeCell ref="AB125:AB127"/>
-    <mergeCell ref="F125:F127"/>
-    <mergeCell ref="H125:H127"/>
-    <mergeCell ref="J125:J127"/>
-    <mergeCell ref="T125:T127"/>
-    <mergeCell ref="P125:P127"/>
-    <mergeCell ref="R125:R127"/>
-    <mergeCell ref="L125:L127"/>
-    <mergeCell ref="N125:N127"/>
-    <mergeCell ref="V125:V127"/>
-    <mergeCell ref="X125:X127"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="AF125:AF127"/>
-    <mergeCell ref="AH125:AH127"/>
-    <mergeCell ref="AJ125:AJ127"/>
-    <mergeCell ref="AL125:AL127"/>
-    <mergeCell ref="AD125:AD127"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -13676,13 +13676,13 @@
       <selection activeCell="I2" sqref="I2:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="17.125" customWidth="1"/>
-    <col min="6" max="6" width="10.25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="10.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B2" s="5" t="s">
         <v>43</v>
       </c>
@@ -13693,7 +13693,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
         <v>18</v>
       </c>
@@ -13707,7 +13707,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="4" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B4" t="s">
         <v>41</v>
       </c>
@@ -13721,7 +13721,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
         <v>46</v>
       </c>
@@ -13735,7 +13735,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="6" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -13749,7 +13749,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="7" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:7" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>42</v>
       </c>
@@ -13763,7 +13763,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="8" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F8" t="s">
         <v>23</v>
       </c>
@@ -13771,7 +13771,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="9" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F9" t="s">
         <v>29</v>
       </c>
@@ -13779,7 +13779,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="10" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F10" t="s">
         <v>25</v>
       </c>
@@ -13787,7 +13787,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F11" t="s">
         <v>33</v>
       </c>
@@ -13795,7 +13795,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="12" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F12" t="s">
         <v>32</v>
       </c>
@@ -13803,7 +13803,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="13" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F13" t="s">
         <v>27</v>
       </c>
@@ -13811,52 +13811,52 @@
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F14" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F15" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="2:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="2:7" x14ac:dyDescent="0.15">
       <c r="F16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="17" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F17" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F18" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F20" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F21" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F22" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="23" spans="6:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="6:6" x14ac:dyDescent="0.15">
       <c r="F23" t="s">
         <v>30</v>
       </c>

</xml_diff>